<commit_message>
NK Product addition static xpath to dynamic xpath corrections
</commit_message>
<xml_diff>
--- a/MyFramework_1/TestData/TD/TD.xlsx
+++ b/MyFramework_1/TestData/TD/TD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NagarajaK\eclipse-workspace\Git_Buckt1\MyFramework_1\TestData\TD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0552C2-559C-4FE5-B3F9-89A92D7D3854}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7864111D-85BB-4E2F-9C12-F07DF1921F9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1C261E98-DB72-41F7-8649-5E6C483EC4A6}"/>
   </bookViews>
@@ -179,9 +179,6 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>ViewSonic VX2757-MHD - LED monitor - Full HD (1080p) - 27</t>
-  </si>
-  <si>
     <t>T24i-20(A20238FT0)23.8 inch Monitor-HDMI</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>StarTech.com Portable USB C Multiport Video Adapter - 4k HDMI or VGA, USB 3.0</t>
+  </si>
+  <si>
+    <t>ViewSonic VX2757-MHD - LED monitor - Full HD (1080p) - 27"</t>
   </si>
 </sst>
 </file>
@@ -636,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9213F3DC-B182-452E-AF46-9D4704FF2230}">
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -754,20 +754,17 @@
       <c r="K2" t="s">
         <v>34</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O2" t="s">
+        <v>49</v>
+      </c>
+      <c r="P2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U2" t="s">
         <v>47</v>
-      </c>
-      <c r="M2" t="s">
-        <v>48</v>
-      </c>
-      <c r="N2" t="s">
-        <v>49</v>
-      </c>
-      <c r="O2" t="s">
-        <v>50</v>
-      </c>
-      <c r="P2" t="s">
-        <v>51</v>
       </c>
       <c r="V2" t="s">
         <v>45</v>
@@ -811,19 +808,19 @@
         <v>34</v>
       </c>
       <c r="L3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" t="s">
         <v>52</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>53</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
+        <v>55</v>
+      </c>
+      <c r="P3" t="s">
         <v>54</v>
-      </c>
-      <c r="O3" t="s">
-        <v>56</v>
-      </c>
-      <c r="P3" t="s">
-        <v>55</v>
       </c>
       <c r="V3" t="s">
         <v>45</v>
@@ -867,19 +864,19 @@
         <v>34</v>
       </c>
       <c r="L4" t="s">
+        <v>56</v>
+      </c>
+      <c r="M4" t="s">
         <v>57</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>58</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>59</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>60</v>
-      </c>
-      <c r="P4" t="s">
-        <v>61</v>
       </c>
       <c r="V4" t="s">
         <v>45</v>
@@ -923,16 +920,16 @@
         <v>34</v>
       </c>
       <c r="L5" t="s">
+        <v>61</v>
+      </c>
+      <c r="M5" t="s">
         <v>62</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>63</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>64</v>
-      </c>
-      <c r="O5" t="s">
-        <v>65</v>
       </c>
       <c r="V5" t="s">
         <v>45</v>
@@ -1337,9 +1334,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE1DBCE9-6DD9-48B4-AE77-F594AF59EC82}">
-  <dimension ref="A1:X5"/>
+  <dimension ref="A1:X8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1606,6 +1605,11 @@
         <v>44</v>
       </c>
     </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="M8" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
City, ST, Zip segregation
</commit_message>
<xml_diff>
--- a/MyFramework_1/TestData/TD/TD.xlsx
+++ b/MyFramework_1/TestData/TD/TD.xlsx
@@ -3,22 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NagarajaK\eclipse-workspace\Git_Buckt1\MyFramework_1\TestData\TD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NagarajaK\eclipse-workspace\selBasic\TestData\TD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6B96FF-A7C5-48B0-915C-9DC4555A0B86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72E78EF-20D7-40C0-AD7B-D8FAA078DD50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1C261E98-DB72-41F7-8649-5E6C483EC4A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1_bkp" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="65">
   <si>
     <t>Date</t>
   </si>
@@ -139,9 +139,6 @@
     <t>Apple USB C Charger cable</t>
   </si>
   <si>
-    <t>11/07/2020 13:27:05</t>
-  </si>
-  <si>
     <t>Branch - Office Supplies Requisiton Template.xlsx</t>
   </si>
   <si>
@@ -163,19 +160,83 @@
     <t>Branch - Office Supplies Requisiton Template3.xlsx</t>
   </si>
   <si>
-    <t>ViewSonic VX2757-MHD - LED monitor - Full HD (1080p) - 27"</t>
-  </si>
-  <si>
-    <t>96W USB-C Power Adapter MacBook Pro + USB-C Charge Cable (2M) Bundle</t>
-  </si>
-  <si>
-    <t>StarTech.com Portable USB C Multiport Video Adapter - 4k HDMI or VGA, USB 3.0</t>
+    <t>11/05/2020 20:10:43</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>ZIP</t>
+  </si>
+  <si>
+    <t>Morisville,NC,27560</t>
+  </si>
+  <si>
+    <t>11/07/2020 18:18:00</t>
+  </si>
+  <si>
+    <t>Morisville</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>27560</t>
+  </si>
+  <si>
+    <t>118800</t>
+  </si>
+  <si>
+    <t>Noorulla Khan</t>
+  </si>
+  <si>
+    <t>600, John Doe Drive</t>
+  </si>
+  <si>
+    <t>Cary,North Carolina,27519-0005</t>
+  </si>
+  <si>
+    <t>noorullak@in.ibm.com</t>
+  </si>
+  <si>
+    <t>919 450 4444</t>
+  </si>
+  <si>
+    <t>P K Bhat</t>
+  </si>
+  <si>
+    <t>pkbhat@in.ibm.com</t>
+  </si>
+  <si>
+    <t>Cary</t>
+  </si>
+  <si>
+    <t>North Carolina</t>
+  </si>
+  <si>
+    <t>27519-0005</t>
+  </si>
+  <si>
+    <t>Morisville,North Carolina,27560</t>
+  </si>
+  <si>
+    <t>Morisville,North carolina,27560</t>
+  </si>
+  <si>
+    <t>North carolina</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -251,10 +312,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,19 +631,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9213F3DC-B182-452E-AF46-9D4704FF2230}">
-  <dimension ref="A1:X5"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.26953125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.453125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -651,13 +713,22 @@
       <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="Y1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1.0</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
@@ -672,7 +743,7 @@
         <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="H2" t="s">
         <v>28</v>
@@ -687,65 +758,97 @@
         <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="M2" t="s">
-        <v>43</v>
-      </c>
-      <c r="N2" t="s">
-        <v>44</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
       <c r="V2" t="s">
+        <v>47</v>
+      </c>
+      <c r="X2" t="s">
         <v>34</v>
       </c>
-      <c r="X2" t="s">
-        <v>35</v>
+      <c r="Y2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2.0</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="I3" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="J3" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="K3" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="L3" t="s">
         <v>32</v>
       </c>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3"/>
       <c r="V3" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="X3" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3.0</v>
       </c>
       <c r="C4" t="s">
         <v>23</v>
@@ -754,13 +857,13 @@
         <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4" t="s">
         <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="H4" t="s">
         <v>28</v>
@@ -789,16 +892,30 @@
       <c r="P4" t="s">
         <v>33</v>
       </c>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+      <c r="U4"/>
       <c r="V4" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="X4" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>4</v>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4.0</v>
       </c>
       <c r="C5" t="s">
         <v>23</v>
@@ -807,13 +924,13 @@
         <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
         <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="H5" t="s">
         <v>28</v>
@@ -836,11 +953,27 @@
       <c r="N5" t="s">
         <v>32</v>
       </c>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5"/>
+      <c r="U5"/>
       <c r="V5" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="X5" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -851,13 +984,292 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F040DFB-EF58-4811-8F23-96D87781F8F2}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38F31BAD-4420-43C5-ACD9-AEE51E1E5E10}">
+  <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.26953125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.453125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" t="s">
+        <v>33</v>
+      </c>
+      <c r="V2" t="s">
+        <v>41</v>
+      </c>
+      <c r="X2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" t="s">
+        <v>32</v>
+      </c>
+      <c r="V3" t="s">
+        <v>41</v>
+      </c>
+      <c r="X3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P4" t="s">
+        <v>33</v>
+      </c>
+      <c r="V4" t="s">
+        <v>41</v>
+      </c>
+      <c r="X4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V5" t="s">
+        <v>41</v>
+      </c>
+      <c r="X5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Invalid Product handler, status update, cart clearing
</commit_message>
<xml_diff>
--- a/MyFramework_1/TestData/TD/TD.xlsx
+++ b/MyFramework_1/TestData/TD/TD.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DeveshBhardwaj\Documents\Devesh\development\GIT BOND\MyFramework_1\TestData\TD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NagarajaK\eclipse-workspace\Git_Buckt1\MyFramework_1\TestData\TD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C321771-9B20-4CD6-87DF-B8BCC2924B96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD863E3-C1C6-48C5-B471-0073B540A21C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1C261E98-DB72-41F7-8649-5E6C483EC4A6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1C261E98-DB72-41F7-8649-5E6C483EC4A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="70">
   <si>
     <t>Date</t>
   </si>
@@ -239,12 +239,19 @@
   </si>
   <si>
     <t>27560-1243</t>
+  </si>
+  <si>
+    <t>Invalid Product exist</t>
+  </si>
+  <si>
+    <t>EVOLVE 65 WIRELESS BLUETOOTH SINGLE EAR HEADSET</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -642,16 +649,16 @@
   <dimension ref="A1:AA5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.453125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -734,10 +741,13 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
       <c r="C2" t="s">
         <v>23</v>
       </c>
@@ -768,6 +778,9 @@
       <c r="L2" t="s">
         <v>65</v>
       </c>
+      <c r="M2" t="s">
+        <v>32</v>
+      </c>
       <c r="V2" t="s">
         <v>47</v>
       </c>
@@ -784,10 +797,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
       <c r="C3" t="s">
         <v>23</v>
       </c>
@@ -815,6 +831,9 @@
       <c r="K3" t="s">
         <v>58</v>
       </c>
+      <c r="L3" t="s">
+        <v>32</v>
+      </c>
       <c r="M3" t="s">
         <v>66</v>
       </c>
@@ -834,10 +853,13 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
       <c r="C4" t="s">
         <v>23</v>
       </c>
@@ -865,6 +887,9 @@
       <c r="K4" t="s">
         <v>31</v>
       </c>
+      <c r="L4" t="s">
+        <v>32</v>
+      </c>
       <c r="M4" t="s">
         <v>33</v>
       </c>
@@ -893,7 +918,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -924,11 +949,8 @@
       <c r="K5" t="s">
         <v>31</v>
       </c>
-      <c r="M5" t="s">
-        <v>33</v>
-      </c>
-      <c r="N5" t="s">
-        <v>32</v>
+      <c r="L5" t="s">
+        <v>69</v>
       </c>
       <c r="V5" t="s">
         <v>47</v>
@@ -961,13 +983,13 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.453125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1041,7 +1063,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1088,7 +1110,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1132,7 +1154,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1188,7 +1210,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
amount check and wrong adderess update 11/10
</commit_message>
<xml_diff>
--- a/MyFramework_1/TestData/TD/TD.xlsx
+++ b/MyFramework_1/TestData/TD/TD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DeveshBhardwaj\Documents\Devesh\development\GIT BOND 3\MyFramework_1\TestData\TD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5795B5-CCF2-4DCF-83FB-D6BE5CD58F3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC72A2B-58B3-456A-9D9A-FB90E53CA92A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1C261E98-DB72-41F7-8649-5E6C483EC4A6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="70">
   <si>
     <t>Date</t>
   </si>
@@ -187,9 +187,6 @@
     <t>NC</t>
   </si>
   <si>
-    <t>27560</t>
-  </si>
-  <si>
     <t>118800</t>
   </si>
   <si>
@@ -223,25 +220,31 @@
     <t>ViewSonic VX2757-MHD - LED monitor - Full HD (1080p) - 27"</t>
   </si>
   <si>
+    <t>Declined -- Total amount greater than $150.00</t>
+  </si>
+  <si>
+    <t>Apple Magic Keyboard - keyboard - US</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>abcde</t>
+  </si>
+  <si>
+    <t>Wrong address provided</t>
+  </si>
+  <si>
+    <t>27560-0001</t>
+  </si>
+  <si>
     <t>Wrong product added for Submission</t>
   </si>
   <si>
-    <t>Declined -- Total amount greater than $150.00</t>
-  </si>
-  <si>
-    <t>Apple Magic Keyboard - keyboard - US</t>
-  </si>
-  <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>abcd</t>
-  </si>
-  <si>
-    <t>abcde</t>
-  </si>
-  <si>
-    <t>Wrong address provided</t>
+    <t>Submission completed with order number: Request details    /    PR458767</t>
   </si>
 </sst>
 </file>
@@ -646,7 +649,7 @@
   <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -744,7 +747,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
@@ -753,7 +756,7 @@
         <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F2" t="s">
         <v>26</v>
@@ -774,7 +777,7 @@
         <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="V2" t="s">
         <v>47</v>
@@ -789,7 +792,7 @@
         <v>49</v>
       </c>
       <c r="AA2" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.3">
@@ -797,37 +800,37 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
       </c>
       <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" t="s">
         <v>51</v>
       </c>
-      <c r="E3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>52</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>53</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>54</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>55</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>56</v>
       </c>
-      <c r="K3" t="s">
-        <v>57</v>
-      </c>
       <c r="L3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="V3" t="s">
         <v>47</v>
@@ -836,13 +839,13 @@
         <v>36</v>
       </c>
       <c r="Y3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z3" t="s">
         <v>58</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>59</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.3">
@@ -850,37 +853,37 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s">
         <v>23</v>
       </c>
       <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" t="s">
         <v>51</v>
       </c>
-      <c r="E4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>52</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>53</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>54</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>55</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>56</v>
       </c>
-      <c r="K4" t="s">
-        <v>57</v>
-      </c>
       <c r="L4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="V4" t="s">
         <v>47</v>
@@ -889,13 +892,13 @@
         <v>36</v>
       </c>
       <c r="Y4" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z4" t="s">
         <v>58</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>59</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cost center and deliver to name update 11/10
</commit_message>
<xml_diff>
--- a/MyFramework_1/TestData/TD/TD.xlsx
+++ b/MyFramework_1/TestData/TD/TD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DeveshBhardwaj\Documents\Devesh\development\GIT BOND 3\MyFramework_1\TestData\TD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC72A2B-58B3-456A-9D9A-FB90E53CA92A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5A0CD2-407D-4C9F-824D-C88779C6F124}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1C261E98-DB72-41F7-8649-5E6C483EC4A6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="80">
   <si>
     <t>Date</t>
   </si>
@@ -241,10 +241,40 @@
     <t>27560-0001</t>
   </si>
   <si>
+    <t>Submission completed with order number: Request details    /    PR459290</t>
+  </si>
+  <si>
+    <t>abc1</t>
+  </si>
+  <si>
+    <t>Submission completed with order number: Request details    /    PR459320</t>
+  </si>
+  <si>
+    <t>Submission completed with order number: Request details    /    PR459324</t>
+  </si>
+  <si>
+    <t>Submission completed with order number: Request details    /    PR459347</t>
+  </si>
+  <si>
+    <t>Submission completed with order number: Request details    /    PR459350</t>
+  </si>
+  <si>
     <t>Wrong product added for Submission</t>
   </si>
   <si>
-    <t>Submission completed with order number: Request details    /    PR458767</t>
+    <t>Submission completed with order number: Request details    /    PR459413</t>
+  </si>
+  <si>
+    <t>Submission completed with order number: Request details    /    PR459420</t>
+  </si>
+  <si>
+    <t>Submission completed with order number: Request details    /    PR459421</t>
+  </si>
+  <si>
+    <t>Submission completed with order number: Request details    /    PR459423</t>
+  </si>
+  <si>
+    <t>Submission completed with order number: Request details    /    PR459450</t>
   </si>
 </sst>
 </file>
@@ -646,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9213F3DC-B182-452E-AF46-9D4704FF2230}">
-  <dimension ref="A1:AA4"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="AA2" sqref="AA2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -747,7 +777,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
@@ -800,52 +830,52 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H3" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="I3" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="J3" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="K3" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="L3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="V3" t="s">
         <v>47</v>
       </c>
       <c r="X3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Y3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="Z3" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="AA3" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.3">
@@ -853,7 +883,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
         <v>23</v>
@@ -862,7 +892,7 @@
         <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F4" t="s">
         <v>51</v>
@@ -883,7 +913,7 @@
         <v>56</v>
       </c>
       <c r="L4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="V4" t="s">
         <v>47</v>
@@ -898,6 +928,59 @@
         <v>58</v>
       </c>
       <c r="AA4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L5" t="s">
+        <v>62</v>
+      </c>
+      <c r="V5" t="s">
+        <v>47</v>
+      </c>
+      <c r="X5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA5" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
total item count check 1121_1950
</commit_message>
<xml_diff>
--- a/MyFramework_1/TestData/TD/TD.xlsx
+++ b/MyFramework_1/TestData/TD/TD.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="459">
   <si>
     <t>Date</t>
   </si>
@@ -1279,6 +1279,138 @@
   </si>
   <si>
     <t>Run Details</t>
+  </si>
+  <si>
+    <t>11/12/2020</t>
+  </si>
+  <si>
+    <t>01205Q</t>
+  </si>
+  <si>
+    <t>Rajasekaran Periasamy</t>
+  </si>
+  <si>
+    <t>Apt # 204, 144 Galway Drive</t>
+  </si>
+  <si>
+    <t>Mooresville</t>
+  </si>
+  <si>
+    <t>28117-5558</t>
+  </si>
+  <si>
+    <t>raperias@in.ibm.com</t>
+  </si>
+  <si>
+    <t>4693860871</t>
+  </si>
+  <si>
+    <t>Vamsi M Thirumala</t>
+  </si>
+  <si>
+    <t>Vamsi M Thirumala1/India/IBM</t>
+  </si>
+  <si>
+    <t>11/21/2020 17:15:24</t>
+  </si>
+  <si>
+    <t>Branch - Office Supplies Vamsi  v2.0-4.xlsx</t>
+  </si>
+  <si>
+    <t>073574</t>
+  </si>
+  <si>
+    <t>Farid Ahmad</t>
+  </si>
+  <si>
+    <t>2106 Lakeview Drive</t>
+  </si>
+  <si>
+    <t>08859-2252</t>
+  </si>
+  <si>
+    <t>fariahma@in.ibm.com</t>
+  </si>
+  <si>
+    <t>732 397 3266</t>
+  </si>
+  <si>
+    <t>Phani Kiran</t>
+  </si>
+  <si>
+    <t>phanikiran@in.ibm.com</t>
+  </si>
+  <si>
+    <t>Farid Ahmad - Emp Id - 073574 -  11 12 2020.xlsx</t>
+  </si>
+  <si>
+    <t>018594</t>
+  </si>
+  <si>
+    <t>HILLOL MUKHERJEE</t>
+  </si>
+  <si>
+    <t>2330 Pleasant Hill Rd. Apt 20</t>
+  </si>
+  <si>
+    <t>Pleasant Hill</t>
+  </si>
+  <si>
+    <t>94523-3160</t>
+  </si>
+  <si>
+    <t>hilmukhe@in.ibm.com</t>
+  </si>
+  <si>
+    <t>925-914-7904</t>
+  </si>
+  <si>
+    <t>JOYJIT BOSE</t>
+  </si>
+  <si>
+    <t>joyjbose@in.ibm.com</t>
+  </si>
+  <si>
+    <t>StarTech.com USB 3.0 to Gigabit Ethernet Adapter - 10/100/1000 NIC Network Adapt</t>
+  </si>
+  <si>
+    <t>Office Supplies Requisiton_018594_HILLOL MUKHERJEE.xlsx</t>
+  </si>
+  <si>
+    <t>11/21/2020 17:16:20</t>
+  </si>
+  <si>
+    <t>11/21/2020 17:46:07</t>
+  </si>
+  <si>
+    <t>11/21/2020 17:47:04</t>
+  </si>
+  <si>
+    <t>Failed - Submission. Please check if an entry is submitted</t>
+  </si>
+  <si>
+    <t>11/21/2020 17:51:43</t>
+  </si>
+  <si>
+    <t>11/21/2020 17:57:58</t>
+  </si>
+  <si>
+    <t>11/21/2020 17:58:55</t>
+  </si>
+  <si>
+    <t>11/21/2020 18:03:52</t>
+  </si>
+  <si>
+    <t>11/21/2020 18:10:12</t>
+  </si>
+  <si>
+    <t>11/21/2020 18:18:28</t>
+  </si>
+  <si>
+    <t>11/21/2020 18:26:42</t>
+  </si>
+  <si>
+    <t>11/21/2020 19:34:01</t>
   </si>
 </sst>
 </file>
@@ -1669,7 +1801,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9213F3DC-B182-452E-AF46-9D4704FF2230}">
-  <dimension ref="A1:Z36"/>
+  <dimension ref="A1:Z72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
@@ -1783,6 +1915,9 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>450</v>
+      </c>
       <c r="C2" t="s">
         <v>26</v>
       </c>
@@ -2307,6 +2442,9 @@
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>450</v>
+      </c>
       <c r="C12" t="s">
         <v>53</v>
       </c>
@@ -2510,6 +2648,9 @@
       <c r="A16">
         <v>15</v>
       </c>
+      <c r="B16" t="s">
+        <v>450</v>
+      </c>
       <c r="C16" t="s">
         <v>133</v>
       </c>
@@ -2560,6 +2701,9 @@
       <c r="A17">
         <v>16</v>
       </c>
+      <c r="B17" t="s">
+        <v>450</v>
+      </c>
       <c r="C17" t="s">
         <v>165</v>
       </c>
@@ -3545,6 +3689,2070 @@
       </c>
       <c r="Z36" t="s">
         <v>401</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>415</v>
+      </c>
+      <c r="D37" t="s">
+        <v>416</v>
+      </c>
+      <c r="E37" t="s">
+        <v>417</v>
+      </c>
+      <c r="F37" t="s">
+        <v>418</v>
+      </c>
+      <c r="G37" t="s">
+        <v>419</v>
+      </c>
+      <c r="H37" t="s">
+        <v>158</v>
+      </c>
+      <c r="I37" t="s">
+        <v>420</v>
+      </c>
+      <c r="J37" t="s">
+        <v>421</v>
+      </c>
+      <c r="K37" t="s">
+        <v>422</v>
+      </c>
+      <c r="L37" t="s">
+        <v>423</v>
+      </c>
+      <c r="M37" t="s">
+        <v>424</v>
+      </c>
+      <c r="N37" t="s">
+        <v>216</v>
+      </c>
+      <c r="O37" t="s">
+        <v>87</v>
+      </c>
+      <c r="P37"/>
+      <c r="Q37"/>
+      <c r="R37"/>
+      <c r="S37"/>
+      <c r="T37"/>
+      <c r="U37"/>
+      <c r="V37"/>
+      <c r="W37"/>
+      <c r="X37" t="s">
+        <v>425</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37.0</v>
+      </c>
+      <c r="C38" t="s">
+        <v>415</v>
+      </c>
+      <c r="D38" t="s">
+        <v>427</v>
+      </c>
+      <c r="E38" t="s">
+        <v>428</v>
+      </c>
+      <c r="F38" t="s">
+        <v>429</v>
+      </c>
+      <c r="G38" t="s">
+        <v>397</v>
+      </c>
+      <c r="H38" t="s">
+        <v>81</v>
+      </c>
+      <c r="I38" t="s">
+        <v>430</v>
+      </c>
+      <c r="J38" t="s">
+        <v>431</v>
+      </c>
+      <c r="K38" t="s">
+        <v>432</v>
+      </c>
+      <c r="L38" t="s">
+        <v>433</v>
+      </c>
+      <c r="M38" t="s">
+        <v>434</v>
+      </c>
+      <c r="N38" t="s">
+        <v>279</v>
+      </c>
+      <c r="O38"/>
+      <c r="P38"/>
+      <c r="Q38"/>
+      <c r="R38"/>
+      <c r="S38"/>
+      <c r="T38"/>
+      <c r="U38"/>
+      <c r="V38"/>
+      <c r="W38"/>
+      <c r="X38" t="s">
+        <v>425</v>
+      </c>
+      <c r="Z38" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="C39" t="s">
+        <v>415</v>
+      </c>
+      <c r="D39" t="s">
+        <v>436</v>
+      </c>
+      <c r="E39" t="s">
+        <v>437</v>
+      </c>
+      <c r="F39" t="s">
+        <v>438</v>
+      </c>
+      <c r="G39" t="s">
+        <v>439</v>
+      </c>
+      <c r="H39" t="s">
+        <v>170</v>
+      </c>
+      <c r="I39" t="s">
+        <v>440</v>
+      </c>
+      <c r="J39" t="s">
+        <v>441</v>
+      </c>
+      <c r="K39" t="s">
+        <v>442</v>
+      </c>
+      <c r="L39" t="s">
+        <v>443</v>
+      </c>
+      <c r="M39" t="s">
+        <v>444</v>
+      </c>
+      <c r="N39" t="s">
+        <v>37</v>
+      </c>
+      <c r="O39" t="s">
+        <v>445</v>
+      </c>
+      <c r="P39"/>
+      <c r="Q39"/>
+      <c r="R39"/>
+      <c r="S39"/>
+      <c r="T39"/>
+      <c r="U39"/>
+      <c r="V39"/>
+      <c r="W39"/>
+      <c r="X39" t="s">
+        <v>425</v>
+      </c>
+      <c r="Z39" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>415</v>
+      </c>
+      <c r="D40" t="s">
+        <v>416</v>
+      </c>
+      <c r="E40" t="s">
+        <v>417</v>
+      </c>
+      <c r="F40" t="s">
+        <v>418</v>
+      </c>
+      <c r="G40" t="s">
+        <v>419</v>
+      </c>
+      <c r="H40" t="s">
+        <v>158</v>
+      </c>
+      <c r="I40" t="s">
+        <v>420</v>
+      </c>
+      <c r="J40" t="s">
+        <v>421</v>
+      </c>
+      <c r="K40" t="s">
+        <v>422</v>
+      </c>
+      <c r="L40" t="s">
+        <v>423</v>
+      </c>
+      <c r="M40" t="s">
+        <v>424</v>
+      </c>
+      <c r="N40" t="s">
+        <v>216</v>
+      </c>
+      <c r="O40" t="s">
+        <v>87</v>
+      </c>
+      <c r="P40"/>
+      <c r="Q40"/>
+      <c r="R40"/>
+      <c r="S40"/>
+      <c r="T40"/>
+      <c r="U40"/>
+      <c r="V40"/>
+      <c r="W40"/>
+      <c r="X40" t="s">
+        <v>447</v>
+      </c>
+      <c r="Z40" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="C41" t="s">
+        <v>415</v>
+      </c>
+      <c r="D41" t="s">
+        <v>427</v>
+      </c>
+      <c r="E41" t="s">
+        <v>428</v>
+      </c>
+      <c r="F41" t="s">
+        <v>429</v>
+      </c>
+      <c r="G41" t="s">
+        <v>397</v>
+      </c>
+      <c r="H41" t="s">
+        <v>81</v>
+      </c>
+      <c r="I41" t="s">
+        <v>430</v>
+      </c>
+      <c r="J41" t="s">
+        <v>431</v>
+      </c>
+      <c r="K41" t="s">
+        <v>432</v>
+      </c>
+      <c r="L41" t="s">
+        <v>433</v>
+      </c>
+      <c r="M41" t="s">
+        <v>434</v>
+      </c>
+      <c r="N41" t="s">
+        <v>279</v>
+      </c>
+      <c r="O41"/>
+      <c r="P41"/>
+      <c r="Q41"/>
+      <c r="R41"/>
+      <c r="S41"/>
+      <c r="T41"/>
+      <c r="U41"/>
+      <c r="V41"/>
+      <c r="W41"/>
+      <c r="X41" t="s">
+        <v>447</v>
+      </c>
+      <c r="Z41" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="C42" t="s">
+        <v>415</v>
+      </c>
+      <c r="D42" t="s">
+        <v>436</v>
+      </c>
+      <c r="E42" t="s">
+        <v>437</v>
+      </c>
+      <c r="F42" t="s">
+        <v>438</v>
+      </c>
+      <c r="G42" t="s">
+        <v>439</v>
+      </c>
+      <c r="H42" t="s">
+        <v>170</v>
+      </c>
+      <c r="I42" t="s">
+        <v>440</v>
+      </c>
+      <c r="J42" t="s">
+        <v>441</v>
+      </c>
+      <c r="K42" t="s">
+        <v>442</v>
+      </c>
+      <c r="L42" t="s">
+        <v>443</v>
+      </c>
+      <c r="M42" t="s">
+        <v>444</v>
+      </c>
+      <c r="N42" t="s">
+        <v>37</v>
+      </c>
+      <c r="O42" t="s">
+        <v>445</v>
+      </c>
+      <c r="P42"/>
+      <c r="Q42"/>
+      <c r="R42"/>
+      <c r="S42"/>
+      <c r="T42"/>
+      <c r="U42"/>
+      <c r="V42"/>
+      <c r="W42"/>
+      <c r="X42" t="s">
+        <v>447</v>
+      </c>
+      <c r="Z42" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="C43" t="s">
+        <v>415</v>
+      </c>
+      <c r="D43" t="s">
+        <v>416</v>
+      </c>
+      <c r="E43" t="s">
+        <v>417</v>
+      </c>
+      <c r="F43" t="s">
+        <v>418</v>
+      </c>
+      <c r="G43" t="s">
+        <v>419</v>
+      </c>
+      <c r="H43" t="s">
+        <v>158</v>
+      </c>
+      <c r="I43" t="s">
+        <v>420</v>
+      </c>
+      <c r="J43" t="s">
+        <v>421</v>
+      </c>
+      <c r="K43" t="s">
+        <v>422</v>
+      </c>
+      <c r="L43" t="s">
+        <v>423</v>
+      </c>
+      <c r="M43" t="s">
+        <v>424</v>
+      </c>
+      <c r="N43" t="s">
+        <v>216</v>
+      </c>
+      <c r="O43" t="s">
+        <v>87</v>
+      </c>
+      <c r="P43"/>
+      <c r="Q43"/>
+      <c r="R43"/>
+      <c r="S43"/>
+      <c r="T43"/>
+      <c r="U43"/>
+      <c r="V43"/>
+      <c r="W43"/>
+      <c r="X43" t="s">
+        <v>448</v>
+      </c>
+      <c r="Z43" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="C44" t="s">
+        <v>415</v>
+      </c>
+      <c r="D44" t="s">
+        <v>427</v>
+      </c>
+      <c r="E44" t="s">
+        <v>428</v>
+      </c>
+      <c r="F44" t="s">
+        <v>429</v>
+      </c>
+      <c r="G44" t="s">
+        <v>397</v>
+      </c>
+      <c r="H44" t="s">
+        <v>81</v>
+      </c>
+      <c r="I44" t="s">
+        <v>430</v>
+      </c>
+      <c r="J44" t="s">
+        <v>431</v>
+      </c>
+      <c r="K44" t="s">
+        <v>432</v>
+      </c>
+      <c r="L44" t="s">
+        <v>433</v>
+      </c>
+      <c r="M44" t="s">
+        <v>434</v>
+      </c>
+      <c r="N44" t="s">
+        <v>279</v>
+      </c>
+      <c r="O44"/>
+      <c r="P44"/>
+      <c r="Q44"/>
+      <c r="R44"/>
+      <c r="S44"/>
+      <c r="T44"/>
+      <c r="U44"/>
+      <c r="V44"/>
+      <c r="W44"/>
+      <c r="X44" t="s">
+        <v>448</v>
+      </c>
+      <c r="Z44" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="C45" t="s">
+        <v>415</v>
+      </c>
+      <c r="D45" t="s">
+        <v>436</v>
+      </c>
+      <c r="E45" t="s">
+        <v>437</v>
+      </c>
+      <c r="F45" t="s">
+        <v>438</v>
+      </c>
+      <c r="G45" t="s">
+        <v>439</v>
+      </c>
+      <c r="H45" t="s">
+        <v>170</v>
+      </c>
+      <c r="I45" t="s">
+        <v>440</v>
+      </c>
+      <c r="J45" t="s">
+        <v>441</v>
+      </c>
+      <c r="K45" t="s">
+        <v>442</v>
+      </c>
+      <c r="L45" t="s">
+        <v>443</v>
+      </c>
+      <c r="M45" t="s">
+        <v>444</v>
+      </c>
+      <c r="N45" t="s">
+        <v>37</v>
+      </c>
+      <c r="O45" t="s">
+        <v>445</v>
+      </c>
+      <c r="P45"/>
+      <c r="Q45"/>
+      <c r="R45"/>
+      <c r="S45"/>
+      <c r="T45"/>
+      <c r="U45"/>
+      <c r="V45"/>
+      <c r="W45"/>
+      <c r="X45" t="s">
+        <v>448</v>
+      </c>
+      <c r="Z45" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="C46" t="s">
+        <v>415</v>
+      </c>
+      <c r="D46" t="s">
+        <v>416</v>
+      </c>
+      <c r="E46" t="s">
+        <v>417</v>
+      </c>
+      <c r="F46" t="s">
+        <v>418</v>
+      </c>
+      <c r="G46" t="s">
+        <v>419</v>
+      </c>
+      <c r="H46" t="s">
+        <v>158</v>
+      </c>
+      <c r="I46" t="s">
+        <v>420</v>
+      </c>
+      <c r="J46" t="s">
+        <v>421</v>
+      </c>
+      <c r="K46" t="s">
+        <v>422</v>
+      </c>
+      <c r="L46" t="s">
+        <v>423</v>
+      </c>
+      <c r="M46" t="s">
+        <v>424</v>
+      </c>
+      <c r="N46" t="s">
+        <v>216</v>
+      </c>
+      <c r="O46" t="s">
+        <v>87</v>
+      </c>
+      <c r="P46"/>
+      <c r="Q46"/>
+      <c r="R46"/>
+      <c r="S46"/>
+      <c r="T46"/>
+      <c r="U46"/>
+      <c r="V46"/>
+      <c r="W46"/>
+      <c r="X46" t="s">
+        <v>449</v>
+      </c>
+      <c r="Z46" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46.0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>415</v>
+      </c>
+      <c r="D47" t="s">
+        <v>427</v>
+      </c>
+      <c r="E47" t="s">
+        <v>428</v>
+      </c>
+      <c r="F47" t="s">
+        <v>429</v>
+      </c>
+      <c r="G47" t="s">
+        <v>397</v>
+      </c>
+      <c r="H47" t="s">
+        <v>81</v>
+      </c>
+      <c r="I47" t="s">
+        <v>430</v>
+      </c>
+      <c r="J47" t="s">
+        <v>431</v>
+      </c>
+      <c r="K47" t="s">
+        <v>432</v>
+      </c>
+      <c r="L47" t="s">
+        <v>433</v>
+      </c>
+      <c r="M47" t="s">
+        <v>434</v>
+      </c>
+      <c r="N47" t="s">
+        <v>279</v>
+      </c>
+      <c r="O47"/>
+      <c r="P47"/>
+      <c r="Q47"/>
+      <c r="R47"/>
+      <c r="S47"/>
+      <c r="T47"/>
+      <c r="U47"/>
+      <c r="V47"/>
+      <c r="W47"/>
+      <c r="X47" t="s">
+        <v>449</v>
+      </c>
+      <c r="Z47" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="C48" t="s">
+        <v>415</v>
+      </c>
+      <c r="D48" t="s">
+        <v>436</v>
+      </c>
+      <c r="E48" t="s">
+        <v>437</v>
+      </c>
+      <c r="F48" t="s">
+        <v>438</v>
+      </c>
+      <c r="G48" t="s">
+        <v>439</v>
+      </c>
+      <c r="H48" t="s">
+        <v>170</v>
+      </c>
+      <c r="I48" t="s">
+        <v>440</v>
+      </c>
+      <c r="J48" t="s">
+        <v>441</v>
+      </c>
+      <c r="K48" t="s">
+        <v>442</v>
+      </c>
+      <c r="L48" t="s">
+        <v>443</v>
+      </c>
+      <c r="M48" t="s">
+        <v>444</v>
+      </c>
+      <c r="N48" t="s">
+        <v>37</v>
+      </c>
+      <c r="O48" t="s">
+        <v>445</v>
+      </c>
+      <c r="P48"/>
+      <c r="Q48"/>
+      <c r="R48"/>
+      <c r="S48"/>
+      <c r="T48"/>
+      <c r="U48"/>
+      <c r="V48"/>
+      <c r="W48"/>
+      <c r="X48" t="s">
+        <v>449</v>
+      </c>
+      <c r="Z48" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="C49" t="s">
+        <v>415</v>
+      </c>
+      <c r="D49" t="s">
+        <v>416</v>
+      </c>
+      <c r="E49" t="s">
+        <v>417</v>
+      </c>
+      <c r="F49" t="s">
+        <v>418</v>
+      </c>
+      <c r="G49" t="s">
+        <v>419</v>
+      </c>
+      <c r="H49" t="s">
+        <v>158</v>
+      </c>
+      <c r="I49" t="s">
+        <v>420</v>
+      </c>
+      <c r="J49" t="s">
+        <v>421</v>
+      </c>
+      <c r="K49" t="s">
+        <v>422</v>
+      </c>
+      <c r="L49" t="s">
+        <v>423</v>
+      </c>
+      <c r="M49" t="s">
+        <v>424</v>
+      </c>
+      <c r="N49" t="s">
+        <v>216</v>
+      </c>
+      <c r="O49" t="s">
+        <v>87</v>
+      </c>
+      <c r="P49"/>
+      <c r="Q49"/>
+      <c r="R49"/>
+      <c r="S49"/>
+      <c r="T49"/>
+      <c r="U49"/>
+      <c r="V49"/>
+      <c r="W49"/>
+      <c r="X49" t="s">
+        <v>451</v>
+      </c>
+      <c r="Z49" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="C50" t="s">
+        <v>415</v>
+      </c>
+      <c r="D50" t="s">
+        <v>427</v>
+      </c>
+      <c r="E50" t="s">
+        <v>428</v>
+      </c>
+      <c r="F50" t="s">
+        <v>429</v>
+      </c>
+      <c r="G50" t="s">
+        <v>397</v>
+      </c>
+      <c r="H50" t="s">
+        <v>81</v>
+      </c>
+      <c r="I50" t="s">
+        <v>430</v>
+      </c>
+      <c r="J50" t="s">
+        <v>431</v>
+      </c>
+      <c r="K50" t="s">
+        <v>432</v>
+      </c>
+      <c r="L50" t="s">
+        <v>433</v>
+      </c>
+      <c r="M50" t="s">
+        <v>434</v>
+      </c>
+      <c r="N50" t="s">
+        <v>279</v>
+      </c>
+      <c r="O50"/>
+      <c r="P50"/>
+      <c r="Q50"/>
+      <c r="R50"/>
+      <c r="S50"/>
+      <c r="T50"/>
+      <c r="U50"/>
+      <c r="V50"/>
+      <c r="W50"/>
+      <c r="X50" t="s">
+        <v>451</v>
+      </c>
+      <c r="Z50" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="C51" t="s">
+        <v>415</v>
+      </c>
+      <c r="D51" t="s">
+        <v>436</v>
+      </c>
+      <c r="E51" t="s">
+        <v>437</v>
+      </c>
+      <c r="F51" t="s">
+        <v>438</v>
+      </c>
+      <c r="G51" t="s">
+        <v>439</v>
+      </c>
+      <c r="H51" t="s">
+        <v>170</v>
+      </c>
+      <c r="I51" t="s">
+        <v>440</v>
+      </c>
+      <c r="J51" t="s">
+        <v>441</v>
+      </c>
+      <c r="K51" t="s">
+        <v>442</v>
+      </c>
+      <c r="L51" t="s">
+        <v>443</v>
+      </c>
+      <c r="M51" t="s">
+        <v>444</v>
+      </c>
+      <c r="N51" t="s">
+        <v>37</v>
+      </c>
+      <c r="O51" t="s">
+        <v>445</v>
+      </c>
+      <c r="P51"/>
+      <c r="Q51"/>
+      <c r="R51"/>
+      <c r="S51"/>
+      <c r="T51"/>
+      <c r="U51"/>
+      <c r="V51"/>
+      <c r="W51"/>
+      <c r="X51" t="s">
+        <v>451</v>
+      </c>
+      <c r="Z51" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51.0</v>
+      </c>
+      <c r="C52" t="s">
+        <v>415</v>
+      </c>
+      <c r="D52" t="s">
+        <v>416</v>
+      </c>
+      <c r="E52" t="s">
+        <v>417</v>
+      </c>
+      <c r="F52" t="s">
+        <v>418</v>
+      </c>
+      <c r="G52" t="s">
+        <v>419</v>
+      </c>
+      <c r="H52" t="s">
+        <v>158</v>
+      </c>
+      <c r="I52" t="s">
+        <v>420</v>
+      </c>
+      <c r="J52" t="s">
+        <v>421</v>
+      </c>
+      <c r="K52" t="s">
+        <v>422</v>
+      </c>
+      <c r="L52" t="s">
+        <v>423</v>
+      </c>
+      <c r="M52" t="s">
+        <v>424</v>
+      </c>
+      <c r="N52" t="s">
+        <v>216</v>
+      </c>
+      <c r="O52" t="s">
+        <v>87</v>
+      </c>
+      <c r="P52"/>
+      <c r="Q52"/>
+      <c r="R52"/>
+      <c r="S52"/>
+      <c r="T52"/>
+      <c r="U52"/>
+      <c r="V52"/>
+      <c r="W52"/>
+      <c r="X52" t="s">
+        <v>452</v>
+      </c>
+      <c r="Z52" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52.0</v>
+      </c>
+      <c r="C53" t="s">
+        <v>415</v>
+      </c>
+      <c r="D53" t="s">
+        <v>427</v>
+      </c>
+      <c r="E53" t="s">
+        <v>428</v>
+      </c>
+      <c r="F53" t="s">
+        <v>429</v>
+      </c>
+      <c r="G53" t="s">
+        <v>397</v>
+      </c>
+      <c r="H53" t="s">
+        <v>81</v>
+      </c>
+      <c r="I53" t="s">
+        <v>430</v>
+      </c>
+      <c r="J53" t="s">
+        <v>431</v>
+      </c>
+      <c r="K53" t="s">
+        <v>432</v>
+      </c>
+      <c r="L53" t="s">
+        <v>433</v>
+      </c>
+      <c r="M53" t="s">
+        <v>434</v>
+      </c>
+      <c r="N53" t="s">
+        <v>279</v>
+      </c>
+      <c r="O53"/>
+      <c r="P53"/>
+      <c r="Q53"/>
+      <c r="R53"/>
+      <c r="S53"/>
+      <c r="T53"/>
+      <c r="U53"/>
+      <c r="V53"/>
+      <c r="W53"/>
+      <c r="X53" t="s">
+        <v>452</v>
+      </c>
+      <c r="Z53" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>53.0</v>
+      </c>
+      <c r="C54" t="s">
+        <v>415</v>
+      </c>
+      <c r="D54" t="s">
+        <v>436</v>
+      </c>
+      <c r="E54" t="s">
+        <v>437</v>
+      </c>
+      <c r="F54" t="s">
+        <v>438</v>
+      </c>
+      <c r="G54" t="s">
+        <v>439</v>
+      </c>
+      <c r="H54" t="s">
+        <v>170</v>
+      </c>
+      <c r="I54" t="s">
+        <v>440</v>
+      </c>
+      <c r="J54" t="s">
+        <v>441</v>
+      </c>
+      <c r="K54" t="s">
+        <v>442</v>
+      </c>
+      <c r="L54" t="s">
+        <v>443</v>
+      </c>
+      <c r="M54" t="s">
+        <v>444</v>
+      </c>
+      <c r="N54" t="s">
+        <v>37</v>
+      </c>
+      <c r="O54" t="s">
+        <v>445</v>
+      </c>
+      <c r="P54"/>
+      <c r="Q54"/>
+      <c r="R54"/>
+      <c r="S54"/>
+      <c r="T54"/>
+      <c r="U54"/>
+      <c r="V54"/>
+      <c r="W54"/>
+      <c r="X54" t="s">
+        <v>452</v>
+      </c>
+      <c r="Z54" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54.0</v>
+      </c>
+      <c r="C55" t="s">
+        <v>415</v>
+      </c>
+      <c r="D55" t="s">
+        <v>416</v>
+      </c>
+      <c r="E55" t="s">
+        <v>417</v>
+      </c>
+      <c r="F55" t="s">
+        <v>418</v>
+      </c>
+      <c r="G55" t="s">
+        <v>419</v>
+      </c>
+      <c r="H55" t="s">
+        <v>158</v>
+      </c>
+      <c r="I55" t="s">
+        <v>420</v>
+      </c>
+      <c r="J55" t="s">
+        <v>421</v>
+      </c>
+      <c r="K55" t="s">
+        <v>422</v>
+      </c>
+      <c r="L55" t="s">
+        <v>423</v>
+      </c>
+      <c r="M55" t="s">
+        <v>424</v>
+      </c>
+      <c r="N55" t="s">
+        <v>216</v>
+      </c>
+      <c r="O55" t="s">
+        <v>87</v>
+      </c>
+      <c r="P55"/>
+      <c r="Q55"/>
+      <c r="R55"/>
+      <c r="S55"/>
+      <c r="T55"/>
+      <c r="U55"/>
+      <c r="V55"/>
+      <c r="W55"/>
+      <c r="X55" t="s">
+        <v>453</v>
+      </c>
+      <c r="Z55" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55.0</v>
+      </c>
+      <c r="C56" t="s">
+        <v>415</v>
+      </c>
+      <c r="D56" t="s">
+        <v>427</v>
+      </c>
+      <c r="E56" t="s">
+        <v>428</v>
+      </c>
+      <c r="F56" t="s">
+        <v>429</v>
+      </c>
+      <c r="G56" t="s">
+        <v>397</v>
+      </c>
+      <c r="H56" t="s">
+        <v>81</v>
+      </c>
+      <c r="I56" t="s">
+        <v>430</v>
+      </c>
+      <c r="J56" t="s">
+        <v>431</v>
+      </c>
+      <c r="K56" t="s">
+        <v>432</v>
+      </c>
+      <c r="L56" t="s">
+        <v>433</v>
+      </c>
+      <c r="M56" t="s">
+        <v>434</v>
+      </c>
+      <c r="N56" t="s">
+        <v>279</v>
+      </c>
+      <c r="O56"/>
+      <c r="P56"/>
+      <c r="Q56"/>
+      <c r="R56"/>
+      <c r="S56"/>
+      <c r="T56"/>
+      <c r="U56"/>
+      <c r="V56"/>
+      <c r="W56"/>
+      <c r="X56" t="s">
+        <v>453</v>
+      </c>
+      <c r="Z56" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56.0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>415</v>
+      </c>
+      <c r="D57" t="s">
+        <v>436</v>
+      </c>
+      <c r="E57" t="s">
+        <v>437</v>
+      </c>
+      <c r="F57" t="s">
+        <v>438</v>
+      </c>
+      <c r="G57" t="s">
+        <v>439</v>
+      </c>
+      <c r="H57" t="s">
+        <v>170</v>
+      </c>
+      <c r="I57" t="s">
+        <v>440</v>
+      </c>
+      <c r="J57" t="s">
+        <v>441</v>
+      </c>
+      <c r="K57" t="s">
+        <v>442</v>
+      </c>
+      <c r="L57" t="s">
+        <v>443</v>
+      </c>
+      <c r="M57" t="s">
+        <v>444</v>
+      </c>
+      <c r="N57" t="s">
+        <v>37</v>
+      </c>
+      <c r="O57" t="s">
+        <v>445</v>
+      </c>
+      <c r="P57"/>
+      <c r="Q57"/>
+      <c r="R57"/>
+      <c r="S57"/>
+      <c r="T57"/>
+      <c r="U57"/>
+      <c r="V57"/>
+      <c r="W57"/>
+      <c r="X57" t="s">
+        <v>453</v>
+      </c>
+      <c r="Z57" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57.0</v>
+      </c>
+      <c r="C58" t="s">
+        <v>415</v>
+      </c>
+      <c r="D58" t="s">
+        <v>416</v>
+      </c>
+      <c r="E58" t="s">
+        <v>417</v>
+      </c>
+      <c r="F58" t="s">
+        <v>418</v>
+      </c>
+      <c r="G58" t="s">
+        <v>419</v>
+      </c>
+      <c r="H58" t="s">
+        <v>158</v>
+      </c>
+      <c r="I58" t="s">
+        <v>420</v>
+      </c>
+      <c r="J58" t="s">
+        <v>421</v>
+      </c>
+      <c r="K58" t="s">
+        <v>422</v>
+      </c>
+      <c r="L58" t="s">
+        <v>423</v>
+      </c>
+      <c r="M58" t="s">
+        <v>424</v>
+      </c>
+      <c r="N58" t="s">
+        <v>216</v>
+      </c>
+      <c r="O58" t="s">
+        <v>87</v>
+      </c>
+      <c r="P58"/>
+      <c r="Q58"/>
+      <c r="R58"/>
+      <c r="S58"/>
+      <c r="T58"/>
+      <c r="U58"/>
+      <c r="V58"/>
+      <c r="W58"/>
+      <c r="X58" t="s">
+        <v>454</v>
+      </c>
+      <c r="Z58" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58.0</v>
+      </c>
+      <c r="C59" t="s">
+        <v>415</v>
+      </c>
+      <c r="D59" t="s">
+        <v>427</v>
+      </c>
+      <c r="E59" t="s">
+        <v>428</v>
+      </c>
+      <c r="F59" t="s">
+        <v>429</v>
+      </c>
+      <c r="G59" t="s">
+        <v>397</v>
+      </c>
+      <c r="H59" t="s">
+        <v>81</v>
+      </c>
+      <c r="I59" t="s">
+        <v>430</v>
+      </c>
+      <c r="J59" t="s">
+        <v>431</v>
+      </c>
+      <c r="K59" t="s">
+        <v>432</v>
+      </c>
+      <c r="L59" t="s">
+        <v>433</v>
+      </c>
+      <c r="M59" t="s">
+        <v>434</v>
+      </c>
+      <c r="N59" t="s">
+        <v>279</v>
+      </c>
+      <c r="O59"/>
+      <c r="P59"/>
+      <c r="Q59"/>
+      <c r="R59"/>
+      <c r="S59"/>
+      <c r="T59"/>
+      <c r="U59"/>
+      <c r="V59"/>
+      <c r="W59"/>
+      <c r="X59" t="s">
+        <v>454</v>
+      </c>
+      <c r="Z59" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59.0</v>
+      </c>
+      <c r="C60" t="s">
+        <v>415</v>
+      </c>
+      <c r="D60" t="s">
+        <v>436</v>
+      </c>
+      <c r="E60" t="s">
+        <v>437</v>
+      </c>
+      <c r="F60" t="s">
+        <v>438</v>
+      </c>
+      <c r="G60" t="s">
+        <v>439</v>
+      </c>
+      <c r="H60" t="s">
+        <v>170</v>
+      </c>
+      <c r="I60" t="s">
+        <v>440</v>
+      </c>
+      <c r="J60" t="s">
+        <v>441</v>
+      </c>
+      <c r="K60" t="s">
+        <v>442</v>
+      </c>
+      <c r="L60" t="s">
+        <v>443</v>
+      </c>
+      <c r="M60" t="s">
+        <v>444</v>
+      </c>
+      <c r="N60" t="s">
+        <v>37</v>
+      </c>
+      <c r="O60" t="s">
+        <v>445</v>
+      </c>
+      <c r="P60"/>
+      <c r="Q60"/>
+      <c r="R60"/>
+      <c r="S60"/>
+      <c r="T60"/>
+      <c r="U60"/>
+      <c r="V60"/>
+      <c r="W60"/>
+      <c r="X60" t="s">
+        <v>454</v>
+      </c>
+      <c r="Z60" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60.0</v>
+      </c>
+      <c r="C61" t="s">
+        <v>415</v>
+      </c>
+      <c r="D61" t="s">
+        <v>416</v>
+      </c>
+      <c r="E61" t="s">
+        <v>417</v>
+      </c>
+      <c r="F61" t="s">
+        <v>418</v>
+      </c>
+      <c r="G61" t="s">
+        <v>419</v>
+      </c>
+      <c r="H61" t="s">
+        <v>158</v>
+      </c>
+      <c r="I61" t="s">
+        <v>420</v>
+      </c>
+      <c r="J61" t="s">
+        <v>421</v>
+      </c>
+      <c r="K61" t="s">
+        <v>422</v>
+      </c>
+      <c r="L61" t="s">
+        <v>423</v>
+      </c>
+      <c r="M61" t="s">
+        <v>424</v>
+      </c>
+      <c r="N61" t="s">
+        <v>216</v>
+      </c>
+      <c r="O61" t="s">
+        <v>87</v>
+      </c>
+      <c r="P61"/>
+      <c r="Q61"/>
+      <c r="R61"/>
+      <c r="S61"/>
+      <c r="T61"/>
+      <c r="U61"/>
+      <c r="V61"/>
+      <c r="W61"/>
+      <c r="X61" t="s">
+        <v>455</v>
+      </c>
+      <c r="Z61" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61.0</v>
+      </c>
+      <c r="C62" t="s">
+        <v>415</v>
+      </c>
+      <c r="D62" t="s">
+        <v>427</v>
+      </c>
+      <c r="E62" t="s">
+        <v>428</v>
+      </c>
+      <c r="F62" t="s">
+        <v>429</v>
+      </c>
+      <c r="G62" t="s">
+        <v>397</v>
+      </c>
+      <c r="H62" t="s">
+        <v>81</v>
+      </c>
+      <c r="I62" t="s">
+        <v>430</v>
+      </c>
+      <c r="J62" t="s">
+        <v>431</v>
+      </c>
+      <c r="K62" t="s">
+        <v>432</v>
+      </c>
+      <c r="L62" t="s">
+        <v>433</v>
+      </c>
+      <c r="M62" t="s">
+        <v>434</v>
+      </c>
+      <c r="N62" t="s">
+        <v>279</v>
+      </c>
+      <c r="O62"/>
+      <c r="P62"/>
+      <c r="Q62"/>
+      <c r="R62"/>
+      <c r="S62"/>
+      <c r="T62"/>
+      <c r="U62"/>
+      <c r="V62"/>
+      <c r="W62"/>
+      <c r="X62" t="s">
+        <v>455</v>
+      </c>
+      <c r="Z62" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62.0</v>
+      </c>
+      <c r="C63" t="s">
+        <v>415</v>
+      </c>
+      <c r="D63" t="s">
+        <v>436</v>
+      </c>
+      <c r="E63" t="s">
+        <v>437</v>
+      </c>
+      <c r="F63" t="s">
+        <v>438</v>
+      </c>
+      <c r="G63" t="s">
+        <v>439</v>
+      </c>
+      <c r="H63" t="s">
+        <v>170</v>
+      </c>
+      <c r="I63" t="s">
+        <v>440</v>
+      </c>
+      <c r="J63" t="s">
+        <v>441</v>
+      </c>
+      <c r="K63" t="s">
+        <v>442</v>
+      </c>
+      <c r="L63" t="s">
+        <v>443</v>
+      </c>
+      <c r="M63" t="s">
+        <v>444</v>
+      </c>
+      <c r="N63" t="s">
+        <v>37</v>
+      </c>
+      <c r="O63" t="s">
+        <v>445</v>
+      </c>
+      <c r="P63"/>
+      <c r="Q63"/>
+      <c r="R63"/>
+      <c r="S63"/>
+      <c r="T63"/>
+      <c r="U63"/>
+      <c r="V63"/>
+      <c r="W63"/>
+      <c r="X63" t="s">
+        <v>455</v>
+      </c>
+      <c r="Z63" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63.0</v>
+      </c>
+      <c r="C64" t="s">
+        <v>415</v>
+      </c>
+      <c r="D64" t="s">
+        <v>416</v>
+      </c>
+      <c r="E64" t="s">
+        <v>417</v>
+      </c>
+      <c r="F64" t="s">
+        <v>418</v>
+      </c>
+      <c r="G64" t="s">
+        <v>419</v>
+      </c>
+      <c r="H64" t="s">
+        <v>158</v>
+      </c>
+      <c r="I64" t="s">
+        <v>420</v>
+      </c>
+      <c r="J64" t="s">
+        <v>421</v>
+      </c>
+      <c r="K64" t="s">
+        <v>422</v>
+      </c>
+      <c r="L64" t="s">
+        <v>423</v>
+      </c>
+      <c r="M64" t="s">
+        <v>424</v>
+      </c>
+      <c r="N64" t="s">
+        <v>216</v>
+      </c>
+      <c r="O64" t="s">
+        <v>87</v>
+      </c>
+      <c r="P64"/>
+      <c r="Q64"/>
+      <c r="R64"/>
+      <c r="S64"/>
+      <c r="T64"/>
+      <c r="U64"/>
+      <c r="V64"/>
+      <c r="W64"/>
+      <c r="X64" t="s">
+        <v>456</v>
+      </c>
+      <c r="Z64" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>64.0</v>
+      </c>
+      <c r="C65" t="s">
+        <v>415</v>
+      </c>
+      <c r="D65" t="s">
+        <v>427</v>
+      </c>
+      <c r="E65" t="s">
+        <v>428</v>
+      </c>
+      <c r="F65" t="s">
+        <v>429</v>
+      </c>
+      <c r="G65" t="s">
+        <v>397</v>
+      </c>
+      <c r="H65" t="s">
+        <v>81</v>
+      </c>
+      <c r="I65" t="s">
+        <v>430</v>
+      </c>
+      <c r="J65" t="s">
+        <v>431</v>
+      </c>
+      <c r="K65" t="s">
+        <v>432</v>
+      </c>
+      <c r="L65" t="s">
+        <v>433</v>
+      </c>
+      <c r="M65" t="s">
+        <v>434</v>
+      </c>
+      <c r="N65" t="s">
+        <v>279</v>
+      </c>
+      <c r="O65"/>
+      <c r="P65"/>
+      <c r="Q65"/>
+      <c r="R65"/>
+      <c r="S65"/>
+      <c r="T65"/>
+      <c r="U65"/>
+      <c r="V65"/>
+      <c r="W65"/>
+      <c r="X65" t="s">
+        <v>456</v>
+      </c>
+      <c r="Z65" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>65.0</v>
+      </c>
+      <c r="C66" t="s">
+        <v>415</v>
+      </c>
+      <c r="D66" t="s">
+        <v>436</v>
+      </c>
+      <c r="E66" t="s">
+        <v>437</v>
+      </c>
+      <c r="F66" t="s">
+        <v>438</v>
+      </c>
+      <c r="G66" t="s">
+        <v>439</v>
+      </c>
+      <c r="H66" t="s">
+        <v>170</v>
+      </c>
+      <c r="I66" t="s">
+        <v>440</v>
+      </c>
+      <c r="J66" t="s">
+        <v>441</v>
+      </c>
+      <c r="K66" t="s">
+        <v>442</v>
+      </c>
+      <c r="L66" t="s">
+        <v>443</v>
+      </c>
+      <c r="M66" t="s">
+        <v>444</v>
+      </c>
+      <c r="N66" t="s">
+        <v>37</v>
+      </c>
+      <c r="O66" t="s">
+        <v>445</v>
+      </c>
+      <c r="P66"/>
+      <c r="Q66"/>
+      <c r="R66"/>
+      <c r="S66"/>
+      <c r="T66"/>
+      <c r="U66"/>
+      <c r="V66"/>
+      <c r="W66"/>
+      <c r="X66" t="s">
+        <v>456</v>
+      </c>
+      <c r="Z66" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="C67" t="s">
+        <v>415</v>
+      </c>
+      <c r="D67" t="s">
+        <v>416</v>
+      </c>
+      <c r="E67" t="s">
+        <v>417</v>
+      </c>
+      <c r="F67" t="s">
+        <v>418</v>
+      </c>
+      <c r="G67" t="s">
+        <v>419</v>
+      </c>
+      <c r="H67" t="s">
+        <v>158</v>
+      </c>
+      <c r="I67" t="s">
+        <v>420</v>
+      </c>
+      <c r="J67" t="s">
+        <v>421</v>
+      </c>
+      <c r="K67" t="s">
+        <v>422</v>
+      </c>
+      <c r="L67" t="s">
+        <v>423</v>
+      </c>
+      <c r="M67" t="s">
+        <v>424</v>
+      </c>
+      <c r="N67" t="s">
+        <v>216</v>
+      </c>
+      <c r="O67" t="s">
+        <v>87</v>
+      </c>
+      <c r="P67"/>
+      <c r="Q67"/>
+      <c r="R67"/>
+      <c r="S67"/>
+      <c r="T67"/>
+      <c r="U67"/>
+      <c r="V67"/>
+      <c r="W67"/>
+      <c r="X67" t="s">
+        <v>457</v>
+      </c>
+      <c r="Z67" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>67.0</v>
+      </c>
+      <c r="C68" t="s">
+        <v>415</v>
+      </c>
+      <c r="D68" t="s">
+        <v>427</v>
+      </c>
+      <c r="E68" t="s">
+        <v>428</v>
+      </c>
+      <c r="F68" t="s">
+        <v>429</v>
+      </c>
+      <c r="G68" t="s">
+        <v>397</v>
+      </c>
+      <c r="H68" t="s">
+        <v>81</v>
+      </c>
+      <c r="I68" t="s">
+        <v>430</v>
+      </c>
+      <c r="J68" t="s">
+        <v>431</v>
+      </c>
+      <c r="K68" t="s">
+        <v>432</v>
+      </c>
+      <c r="L68" t="s">
+        <v>433</v>
+      </c>
+      <c r="M68" t="s">
+        <v>434</v>
+      </c>
+      <c r="N68" t="s">
+        <v>279</v>
+      </c>
+      <c r="O68"/>
+      <c r="P68"/>
+      <c r="Q68"/>
+      <c r="R68"/>
+      <c r="S68"/>
+      <c r="T68"/>
+      <c r="U68"/>
+      <c r="V68"/>
+      <c r="W68"/>
+      <c r="X68" t="s">
+        <v>457</v>
+      </c>
+      <c r="Z68" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>68.0</v>
+      </c>
+      <c r="C69" t="s">
+        <v>415</v>
+      </c>
+      <c r="D69" t="s">
+        <v>436</v>
+      </c>
+      <c r="E69" t="s">
+        <v>437</v>
+      </c>
+      <c r="F69" t="s">
+        <v>438</v>
+      </c>
+      <c r="G69" t="s">
+        <v>439</v>
+      </c>
+      <c r="H69" t="s">
+        <v>170</v>
+      </c>
+      <c r="I69" t="s">
+        <v>440</v>
+      </c>
+      <c r="J69" t="s">
+        <v>441</v>
+      </c>
+      <c r="K69" t="s">
+        <v>442</v>
+      </c>
+      <c r="L69" t="s">
+        <v>443</v>
+      </c>
+      <c r="M69" t="s">
+        <v>444</v>
+      </c>
+      <c r="N69" t="s">
+        <v>37</v>
+      </c>
+      <c r="O69" t="s">
+        <v>445</v>
+      </c>
+      <c r="P69"/>
+      <c r="Q69"/>
+      <c r="R69"/>
+      <c r="S69"/>
+      <c r="T69"/>
+      <c r="U69"/>
+      <c r="V69"/>
+      <c r="W69"/>
+      <c r="X69" t="s">
+        <v>457</v>
+      </c>
+      <c r="Z69" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>69.0</v>
+      </c>
+      <c r="C70" t="s">
+        <v>415</v>
+      </c>
+      <c r="D70" t="s">
+        <v>416</v>
+      </c>
+      <c r="E70" t="s">
+        <v>417</v>
+      </c>
+      <c r="F70" t="s">
+        <v>418</v>
+      </c>
+      <c r="G70" t="s">
+        <v>419</v>
+      </c>
+      <c r="H70" t="s">
+        <v>158</v>
+      </c>
+      <c r="I70" t="s">
+        <v>420</v>
+      </c>
+      <c r="J70" t="s">
+        <v>421</v>
+      </c>
+      <c r="K70" t="s">
+        <v>422</v>
+      </c>
+      <c r="L70" t="s">
+        <v>423</v>
+      </c>
+      <c r="M70" t="s">
+        <v>424</v>
+      </c>
+      <c r="N70" t="s">
+        <v>216</v>
+      </c>
+      <c r="O70" t="s">
+        <v>87</v>
+      </c>
+      <c r="P70"/>
+      <c r="Q70"/>
+      <c r="R70"/>
+      <c r="S70"/>
+      <c r="T70"/>
+      <c r="U70"/>
+      <c r="V70"/>
+      <c r="W70"/>
+      <c r="X70" t="s">
+        <v>458</v>
+      </c>
+      <c r="Z70" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>70.0</v>
+      </c>
+      <c r="C71" t="s">
+        <v>415</v>
+      </c>
+      <c r="D71" t="s">
+        <v>427</v>
+      </c>
+      <c r="E71" t="s">
+        <v>428</v>
+      </c>
+      <c r="F71" t="s">
+        <v>429</v>
+      </c>
+      <c r="G71" t="s">
+        <v>397</v>
+      </c>
+      <c r="H71" t="s">
+        <v>81</v>
+      </c>
+      <c r="I71" t="s">
+        <v>430</v>
+      </c>
+      <c r="J71" t="s">
+        <v>431</v>
+      </c>
+      <c r="K71" t="s">
+        <v>432</v>
+      </c>
+      <c r="L71" t="s">
+        <v>433</v>
+      </c>
+      <c r="M71" t="s">
+        <v>434</v>
+      </c>
+      <c r="N71" t="s">
+        <v>279</v>
+      </c>
+      <c r="O71"/>
+      <c r="P71"/>
+      <c r="Q71"/>
+      <c r="R71"/>
+      <c r="S71"/>
+      <c r="T71"/>
+      <c r="U71"/>
+      <c r="V71"/>
+      <c r="W71"/>
+      <c r="X71" t="s">
+        <v>458</v>
+      </c>
+      <c r="Z71" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>71.0</v>
+      </c>
+      <c r="C72" t="s">
+        <v>415</v>
+      </c>
+      <c r="D72" t="s">
+        <v>436</v>
+      </c>
+      <c r="E72" t="s">
+        <v>437</v>
+      </c>
+      <c r="F72" t="s">
+        <v>438</v>
+      </c>
+      <c r="G72" t="s">
+        <v>439</v>
+      </c>
+      <c r="H72" t="s">
+        <v>170</v>
+      </c>
+      <c r="I72" t="s">
+        <v>440</v>
+      </c>
+      <c r="J72" t="s">
+        <v>441</v>
+      </c>
+      <c r="K72" t="s">
+        <v>442</v>
+      </c>
+      <c r="L72" t="s">
+        <v>443</v>
+      </c>
+      <c r="M72" t="s">
+        <v>444</v>
+      </c>
+      <c r="N72" t="s">
+        <v>37</v>
+      </c>
+      <c r="O72" t="s">
+        <v>445</v>
+      </c>
+      <c r="P72"/>
+      <c r="Q72"/>
+      <c r="R72"/>
+      <c r="S72"/>
+      <c r="T72"/>
+      <c r="U72"/>
+      <c r="V72"/>
+      <c r="W72"/>
+      <c r="X72" t="s">
+        <v>458</v>
+      </c>
+      <c r="Z72" t="s">
+        <v>446</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NK changes wait fix and other changes
</commit_message>
<xml_diff>
--- a/MyFramework_1/TestData/TD/TD.xlsx
+++ b/MyFramework_1/TestData/TD/TD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NagarajaK\eclipse-workspace\Git_Buckt1\MyFramework_1\TestData\TD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BA3600-278E-4156-B075-4F19A056F4F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23074DE2-125D-41DA-BBF8-F689213D8B69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1C261E98-DB72-41F7-8649-5E6C483EC4A6}"/>
+    <workbookView xWindow="20" yWindow="620" windowWidth="19180" windowHeight="10180" xr2:uid="{1C261E98-DB72-41F7-8649-5E6C483EC4A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="439">
   <si>
     <t>Date</t>
   </si>
@@ -1344,34 +1344,13 @@
     <t>Office Supplies Requisiton_018594_HILLOL MUKHERJEE.xlsx</t>
   </si>
   <si>
-    <t>Success - Submission completed with order number: Request details    /    PR470330</t>
-  </si>
-  <si>
-    <t>Success - Submission completed with order number: Request details    /    PR470344</t>
-  </si>
-  <si>
-    <t>Success - Submission completed with order number: Request details    /    PR470354</t>
-  </si>
-  <si>
-    <t>Success - Submission completed with order number: Request details    /    PR470357</t>
-  </si>
-  <si>
-    <t>Failed - Submission. Please check if an entry is submitted</t>
-  </si>
-  <si>
-    <t>Failed -Invalid Product exist :Apple USB-C Charge Cable - USB-C cable - 2 m</t>
-  </si>
-  <si>
-    <t>Success - Submission completed with order number: Request details    /    PR470437</t>
+    <t>Product added to cart- Checkout pending</t>
   </si>
   <si>
     <t xml:space="preserve">Failed -Invalid Product exist : </t>
   </si>
   <si>
-    <t>Failed -Invalid Product exist :T24i-20(A20238FT0)23.8 inch Monitor-HDMI</t>
-  </si>
-  <si>
-    <t>Success - Submission completed with order number: Request details    /    PR470466</t>
+    <t>Failed -Invalid Product exist :StarTech.com Portable USB C Multiport Video Adapter - 4k HDMI or VGA, USB 3.0</t>
   </si>
 </sst>
 </file>
@@ -1764,9 +1743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9213F3DC-B182-452E-AF46-9D4704FF2230}">
   <dimension ref="A1:Z39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B51"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1927,7 +1904,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="C3" t="s">
         <v>40</v>
@@ -1980,7 +1957,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C4" t="s">
         <v>53</v>
@@ -2033,7 +2010,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C5" t="s">
         <v>40</v>
@@ -2083,7 +2060,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C6" t="s">
         <v>76</v>
@@ -2136,7 +2113,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="C7" t="s">
         <v>90</v>
@@ -2189,7 +2166,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="C8" t="s">
         <v>40</v>
@@ -2241,6 +2218,9 @@
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>436</v>
+      </c>
       <c r="C9" t="s">
         <v>90</v>
       </c>
@@ -2291,6 +2271,9 @@
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>436</v>
+      </c>
       <c r="C10" t="s">
         <v>121</v>
       </c>
@@ -2344,6 +2327,9 @@
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11" t="s">
+        <v>436</v>
+      </c>
       <c r="C11" t="s">
         <v>133</v>
       </c>
@@ -2394,6 +2380,9 @@
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>436</v>
+      </c>
       <c r="C12" t="s">
         <v>53</v>
       </c>
@@ -2445,7 +2434,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="C13" t="s">
         <v>76</v>
@@ -2495,7 +2484,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="C14" t="s">
         <v>165</v>
@@ -2547,6 +2536,9 @@
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15" t="s">
+        <v>436</v>
+      </c>
       <c r="C15" t="s">
         <v>165</v>
       </c>
@@ -2598,7 +2590,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="C16" t="s">
         <v>133</v>
@@ -2651,7 +2643,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="C17" t="s">
         <v>165</v>
@@ -2703,6 +2695,9 @@
       <c r="A18">
         <v>17</v>
       </c>
+      <c r="B18" t="s">
+        <v>436</v>
+      </c>
       <c r="C18" t="s">
         <v>40</v>
       </c>
@@ -2753,6 +2748,9 @@
       <c r="A19">
         <v>18</v>
       </c>
+      <c r="B19" t="s">
+        <v>436</v>
+      </c>
       <c r="C19" t="s">
         <v>218</v>
       </c>
@@ -2803,6 +2801,9 @@
       <c r="A20">
         <v>19</v>
       </c>
+      <c r="B20" t="s">
+        <v>436</v>
+      </c>
       <c r="C20" t="s">
         <v>121</v>
       </c>
@@ -2853,6 +2854,9 @@
       <c r="A21">
         <v>20</v>
       </c>
+      <c r="B21" t="s">
+        <v>436</v>
+      </c>
       <c r="C21" t="s">
         <v>133</v>
       </c>
@@ -2900,6 +2904,9 @@
       <c r="A22">
         <v>21</v>
       </c>
+      <c r="B22" t="s">
+        <v>436</v>
+      </c>
       <c r="C22" t="s">
         <v>133</v>
       </c>
@@ -2950,6 +2957,9 @@
       <c r="A23">
         <v>22</v>
       </c>
+      <c r="B23" t="s">
+        <v>436</v>
+      </c>
       <c r="C23" t="s">
         <v>165</v>
       </c>
@@ -3000,6 +3010,9 @@
       <c r="A24">
         <v>23</v>
       </c>
+      <c r="B24" t="s">
+        <v>436</v>
+      </c>
       <c r="C24" t="s">
         <v>53</v>
       </c>
@@ -3050,6 +3063,9 @@
       <c r="A25">
         <v>24</v>
       </c>
+      <c r="B25" t="s">
+        <v>436</v>
+      </c>
       <c r="C25" t="s">
         <v>53</v>
       </c>
@@ -3097,6 +3113,9 @@
       <c r="A26">
         <v>25</v>
       </c>
+      <c r="B26" t="s">
+        <v>436</v>
+      </c>
       <c r="C26" t="s">
         <v>165</v>
       </c>
@@ -3144,6 +3163,9 @@
       <c r="A27">
         <v>26</v>
       </c>
+      <c r="B27" t="s">
+        <v>438</v>
+      </c>
       <c r="C27" t="s">
         <v>53</v>
       </c>
@@ -3197,6 +3219,9 @@
       <c r="A28">
         <v>27</v>
       </c>
+      <c r="B28" t="s">
+        <v>436</v>
+      </c>
       <c r="C28" t="s">
         <v>40</v>
       </c>
@@ -3247,6 +3272,9 @@
       <c r="A29">
         <v>28</v>
       </c>
+      <c r="B29" t="s">
+        <v>436</v>
+      </c>
       <c r="C29" t="s">
         <v>53</v>
       </c>
@@ -3297,6 +3325,9 @@
       <c r="A30">
         <v>29</v>
       </c>
+      <c r="B30" t="s">
+        <v>436</v>
+      </c>
       <c r="C30" t="s">
         <v>165</v>
       </c>
@@ -3344,6 +3375,9 @@
       <c r="A31">
         <v>30</v>
       </c>
+      <c r="B31" t="s">
+        <v>436</v>
+      </c>
       <c r="C31" t="s">
         <v>133</v>
       </c>
@@ -3397,6 +3431,9 @@
       <c r="A32">
         <v>31</v>
       </c>
+      <c r="B32" t="s">
+        <v>436</v>
+      </c>
       <c r="C32" t="s">
         <v>133</v>
       </c>
@@ -3447,6 +3484,9 @@
       <c r="A33">
         <v>32</v>
       </c>
+      <c r="B33" t="s">
+        <v>436</v>
+      </c>
       <c r="C33" t="s">
         <v>121</v>
       </c>
@@ -3497,6 +3537,9 @@
       <c r="A34">
         <v>33</v>
       </c>
+      <c r="B34" t="s">
+        <v>436</v>
+      </c>
       <c r="C34" t="s">
         <v>371</v>
       </c>
@@ -3544,6 +3587,9 @@
       <c r="A35">
         <v>34</v>
       </c>
+      <c r="B35" t="s">
+        <v>436</v>
+      </c>
       <c r="C35" t="s">
         <v>382</v>
       </c>
@@ -3594,6 +3640,9 @@
       <c r="A36">
         <v>35</v>
       </c>
+      <c r="B36" t="s">
+        <v>436</v>
+      </c>
       <c r="C36" t="s">
         <v>40</v>
       </c>
@@ -3694,6 +3743,9 @@
       <c r="A38">
         <v>37</v>
       </c>
+      <c r="B38" t="s">
+        <v>436</v>
+      </c>
       <c r="C38" t="s">
         <v>404</v>
       </c>
@@ -3740,6 +3792,9 @@
     <row r="39" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>436</v>
       </c>
       <c r="C39" t="s">
         <v>404</v>

</xml_diff>